<commit_message>
started new pages for W-183 and W-184
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/tungsten.xlsx
+++ b/levelfiles/spreadsheet/tungsten.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
     <sheet name="187 - primary gammas" sheetId="2" r:id="rId2"/>
+    <sheet name="183 - primary gammas" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>iso</t>
   </si>
@@ -82,15 +83,47 @@
   <si>
     <t>ratio (%)</t>
   </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>to ground = 0.134</t>
+  </si>
+  <si>
+    <t>to ground = 0.97</t>
+  </si>
+  <si>
+    <t>to ground = 0.319</t>
+  </si>
+  <si>
+    <t>to ground = 0.148</t>
+  </si>
+  <si>
+    <t>data from https://escholarship.org/uc/item/26q2x5f0</t>
+  </si>
+  <si>
+    <t>transitions from Sn all dipole transitions</t>
+  </si>
+  <si>
+    <t>major transition</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,15 +152,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -636,10 +672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G311"/>
+  <dimension ref="A1:J313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="F168" sqref="F168"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,9 +684,10 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>9</v>
       </c>
@@ -662,10 +699,10 @@
         <v>11</v>
       </c>
       <c r="G1">
-        <v>18.39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38.090000000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -678,21 +715,33 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>$E$1 - C3</f>
         <v>5466.76</v>
       </c>
+      <c r="B3">
+        <v>2.3E-2</v>
+      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f>100*B3/$G$1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.0383302704121809E-2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">$E$1 - C4</f>
         <v>5389.4710000000005</v>
@@ -704,21 +753,33 @@
         <f t="shared" ref="D4:D67" si="1">100*B4/$G$1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>5320.9120000000003</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="2">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="C5" s="2">
         <v>145.84800000000001</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5883433972171173</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5265.3110000000006</v>
@@ -730,21 +791,33 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>5261.8580000000002</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="C7" s="2">
         <v>204.90199999999999</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2578104489367288</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5163.4070000000002</v>
@@ -757,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>5135.9800000000005</v>
@@ -770,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5116.3290000000006</v>
@@ -783,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>5102.54</v>
@@ -796,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>5056.7</v>
@@ -809,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>5034.4780000000001</v>
@@ -822,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>4956.76</v>
@@ -835,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>4944.6100000000006</v>
@@ -848,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>4928.3100000000004</v>
@@ -978,17 +1051,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>4684.47</v>
       </c>
-      <c r="C26">
+      <c r="B26" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C26" s="2">
         <v>782.29</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="D26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.39380414807035963</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1082,17 +1158,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="34" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>4626.5550000000003</v>
       </c>
-      <c r="C34">
+      <c r="B34" s="2">
+        <v>0.124</v>
+      </c>
+      <c r="C34" s="2">
         <v>840.20500000000004</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="D34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.32554476240483066</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1173,17 +1252,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>4574.83</v>
       </c>
-      <c r="C41">
+      <c r="B41" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="C41" s="2">
         <v>891.93</v>
       </c>
-      <c r="D41">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="D41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.39905487004463108</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1602,17 +1684,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="74" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
         <f t="shared" si="2"/>
         <v>4249.634</v>
       </c>
-      <c r="C74">
+      <c r="B74" s="2">
+        <v>0.115</v>
+      </c>
+      <c r="C74" s="2">
         <v>1217.126</v>
       </c>
-      <c r="D74">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="D74" s="2">
+        <f t="shared" si="3"/>
+        <v>0.30191651352060905</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2876,7 +2961,7 @@
       </c>
       <c r="D171" s="2">
         <f t="shared" si="5"/>
-        <v>0.56008700380641641</v>
+        <v>0.27041218167498027</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -4608,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305">
         <f t="shared" si="8"/>
         <v>2570.2600000000002</v>
@@ -4621,7 +4706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306">
         <f t="shared" si="8"/>
         <v>2557.2600000000002</v>
@@ -4634,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307">
         <f t="shared" si="8"/>
         <v>2536.46</v>
@@ -4647,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308">
         <f t="shared" si="8"/>
         <v>2431.0600000000004</v>
@@ -4660,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309">
         <f t="shared" si="8"/>
         <v>2322.17</v>
@@ -4673,7 +4758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310">
         <f t="shared" si="8"/>
         <v>2290.46</v>
@@ -4686,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311">
         <f t="shared" si="8"/>
         <v>2122.96</v>
@@ -4699,7 +4784,74 @@
         <v>0</v>
       </c>
     </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D313">
+        <f>SUM(D3:D311)</f>
+        <v>5.5972696245733795</v>
+      </c>
+      <c r="E313" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://escholarship.org/uc/item/26q2x5f0"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1">
+        <f>6.19084*1000</f>
+        <v>6190.8399999999992</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1">
+        <v>18.39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://escholarship.org/uc/item/26q2x5f0"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all ENSDF level transition intensities from neutron sep energy
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/tungsten.xlsx
+++ b/levelfiles/spreadsheet/tungsten.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>iso</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>has primary transitions in ENSDF</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>barns</t>
   </si>
 </sst>
 </file>
@@ -6187,10 +6193,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I332"/>
+  <dimension ref="A1:I335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="B224" sqref="B224"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6231,7 +6237,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>18</v>
@@ -6243,14 +6249,13 @@
         <v>6190.8399999999992</v>
       </c>
       <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.45</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <f>100*B3/$G$1</f>
-        <v>2.2647206844489181</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>20</v>
@@ -6258,18 +6263,17 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A258" si="0">$E$1-C4</f>
+        <f t="shared" ref="A4:A260" si="0">$E$1-C4</f>
         <v>6144.3561999999993</v>
       </c>
       <c r="B4" s="2">
-        <v>0.17399999999999999</v>
+        <v>36.9</v>
       </c>
       <c r="C4" s="2">
         <v>46.483800000000002</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D53" si="1">100*B4/$G$1</f>
-        <v>0.87569199798691488</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>28</v>
@@ -6283,13 +6287,12 @@
         <f t="shared" si="0"/>
         <v>6091.7608999999993</v>
       </c>
+      <c r="B5">
+        <v>0.23</v>
+      </c>
       <c r="C5">
         <v>99.079099999999997</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
@@ -6305,10 +6308,6 @@
       <c r="C6">
         <v>207.01140000000001</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="F6" t="s">
         <v>31</v>
       </c>
@@ -6318,13 +6317,12 @@
         <f t="shared" si="0"/>
         <v>5982.0330999999996</v>
       </c>
+      <c r="B7">
+        <v>0.59</v>
+      </c>
       <c r="C7">
         <v>208.80690000000001</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="F7" t="s">
         <v>35</v>
       </c>
@@ -6340,10 +6338,6 @@
       <c r="C8">
         <v>291.72359999999998</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -6353,10 +6347,6 @@
       <c r="C9">
         <v>308.94659999999999</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -6366,10 +6356,6 @@
       <c r="C10">
         <v>309.49200000000002</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -6379,10 +6365,6 @@
       <c r="C11">
         <v>412.09390000000002</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -6392,10 +6374,6 @@
       <c r="C12">
         <v>453.06950000000001</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -6405,10 +6383,6 @@
       <c r="C13">
         <v>475.05</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -6418,10 +6392,6 @@
       <c r="C14">
         <v>485.38</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -6431,10 +6401,6 @@
       <c r="C15">
         <v>533</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -6444,23 +6410,18 @@
       <c r="C16">
         <v>551.24</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>5633.3399999999992</v>
       </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
       <c r="C17">
         <v>557.5</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="I17" t="s">
         <v>51</v>
       </c>
@@ -6473,10 +6434,6 @@
       <c r="C18">
         <v>595.33799999999997</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -6486,10 +6443,6 @@
       <c r="C19">
         <v>622.6</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -6499,23 +6452,18 @@
       <c r="C20">
         <v>631.11</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>5513.1399999999994</v>
       </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
       <c r="C21">
         <v>677.7</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -6525,10 +6473,6 @@
       <c r="C22">
         <v>687.63</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -6538,10 +6482,6 @@
       <c r="C23">
         <v>739.95</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -6551,10 +6491,6 @@
       <c r="C24">
         <v>766.3</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -6564,10 +6500,6 @@
       <c r="C25">
         <v>776.8</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -6577,36 +6509,30 @@
       <c r="C26">
         <v>777</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>5385.94</v>
       </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
       <c r="C27">
         <v>804.9</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>5382.5399999999991</v>
       </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
       <c r="C28">
         <v>808.3</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -6616,10 +6542,6 @@
       <c r="C29">
         <v>816.5</v>
       </c>
-      <c r="D29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -6629,10 +6551,6 @@
       <c r="C30">
         <v>849.94</v>
       </c>
-      <c r="D30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -6642,10 +6560,6 @@
       <c r="C31">
         <v>871.9</v>
       </c>
-      <c r="D31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -6655,10 +6569,6 @@
       <c r="C32">
         <v>899.7</v>
       </c>
-      <c r="D32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -6668,23 +6578,18 @@
       <c r="C33">
         <v>903.50300000000004</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>5281.44</v>
       </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
       <c r="C34">
         <v>909.4</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -6694,10 +6599,6 @@
       <c r="C35">
         <v>914.81</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -6707,62 +6608,54 @@
       <c r="C36">
         <v>926.1</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>5256.1789999999992</v>
       </c>
+      <c r="B37">
+        <v>2.38</v>
+      </c>
       <c r="C37">
         <v>934.66099999999994</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>5249.2399999999989</v>
       </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
       <c r="C38">
         <v>941.6</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>5240.9399999999996</v>
       </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
       <c r="C39">
         <v>949.9</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>5239.5399999999991</v>
       </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
       <c r="C40">
         <v>951.3</v>
       </c>
-      <c r="D40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -6772,10 +6665,6 @@
       <c r="C41">
         <v>956.3</v>
       </c>
-      <c r="D41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -6785,10 +6674,6 @@
       <c r="C42">
         <v>960</v>
       </c>
-      <c r="D42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -6798,10 +6683,6 @@
       <c r="C43">
         <v>963.43</v>
       </c>
-      <c r="D43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -6811,10 +6692,6 @@
       <c r="C44">
         <v>965.13</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -6824,10 +6701,6 @@
       <c r="C45">
         <v>999.6</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -6835,14 +6708,13 @@
         <v>5164.4669999999987</v>
       </c>
       <c r="B46" s="2">
-        <v>0.19</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="C46" s="2">
         <v>1026.373</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="1"/>
-        <v>0.9562154001006542</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -6853,10 +6725,6 @@
       <c r="C47">
         <v>1053.299</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -6866,12 +6734,8 @@
       <c r="C48">
         <v>1061.99</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>5121.4199999999992</v>
@@ -6879,25 +6743,20 @@
       <c r="C49">
         <v>1069.42</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>5094.4399999999987</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
       </c>
       <c r="C50">
         <v>1096.4000000000001</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>5064.6399999999994</v>
@@ -6905,25 +6764,20 @@
       <c r="C51">
         <v>1126.2</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>5040.9299999999994</v>
+      </c>
+      <c r="B52">
+        <v>0.16</v>
       </c>
       <c r="C52">
         <v>1149.9100000000001</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>5034.8399999999992</v>
@@ -6931,12 +6785,8 @@
       <c r="C53">
         <v>1156</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>5022.0999999999995</v>
@@ -6945,16 +6795,19 @@
         <v>1168.74</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>5002.4399999999987</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
       </c>
       <c r="C55">
         <v>1188.4000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>5000.5899999999992</v>
@@ -6963,7 +6816,7 @@
         <v>1190.25</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>4976.5299999999988</v>
@@ -6972,7 +6825,7 @@
         <v>1214.31</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>4967.4399999999987</v>
@@ -6981,16 +6834,19 @@
         <v>1223.4000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>4964.3399999999992</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
       </c>
       <c r="C59">
         <v>1226.5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>4961.5299999999988</v>
@@ -6999,7 +6855,7 @@
         <v>1229.31</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>4929.4399999999987</v>
@@ -7008,16 +6864,19 @@
         <v>1261.4000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>4918.6399999999994</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
       </c>
       <c r="C62">
         <v>1272.2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>4915.6499999999996</v>
@@ -7026,7 +6885,7 @@
         <v>1275.19</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>4909.8399999999992</v>
@@ -7040,6 +6899,9 @@
         <f t="shared" si="0"/>
         <v>4899.1699999999992</v>
       </c>
+      <c r="B65">
+        <v>0.08</v>
+      </c>
       <c r="C65">
         <v>1291.67</v>
       </c>
@@ -7049,6 +6911,9 @@
         <f t="shared" si="0"/>
         <v>4881.4309999999987</v>
       </c>
+      <c r="B66">
+        <v>1.04</v>
+      </c>
       <c r="C66">
         <v>1309.4090000000001</v>
       </c>
@@ -7094,6 +6959,9 @@
         <f t="shared" si="0"/>
         <v>4855.4199999999992</v>
       </c>
+      <c r="B71">
+        <v>0.13</v>
+      </c>
       <c r="C71">
         <v>1335.42</v>
       </c>
@@ -7112,6 +6980,9 @@
         <f t="shared" si="0"/>
         <v>4818.6099999999988</v>
       </c>
+      <c r="B73">
+        <v>0.1</v>
+      </c>
       <c r="C73">
         <v>1372.23</v>
       </c>
@@ -7157,6 +7028,9 @@
         <f t="shared" si="0"/>
         <v>4777.9399999999987</v>
       </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
       <c r="C78">
         <v>1412.9</v>
       </c>
@@ -7166,6 +7040,9 @@
         <f t="shared" si="0"/>
         <v>4773.24</v>
       </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
       <c r="C79">
         <v>1417.6</v>
       </c>
@@ -7184,6 +7061,9 @@
         <f t="shared" si="0"/>
         <v>4753.4199999999992</v>
       </c>
+      <c r="B81">
+        <v>0.27</v>
+      </c>
       <c r="C81">
         <v>1437.42</v>
       </c>
@@ -7211,6 +7091,9 @@
         <f t="shared" si="0"/>
         <v>4727.6599999999989</v>
       </c>
+      <c r="B84">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="C84">
         <v>1463.18</v>
       </c>
@@ -7229,6 +7112,9 @@
         <f t="shared" si="0"/>
         <v>4719.7899999999991</v>
       </c>
+      <c r="B86">
+        <v>3.61</v>
+      </c>
       <c r="C86">
         <v>1471.05</v>
       </c>
@@ -7247,6 +7133,9 @@
         <f t="shared" si="0"/>
         <v>4705.3899999999994</v>
       </c>
+      <c r="B88">
+        <v>0.1</v>
+      </c>
       <c r="C88">
         <v>1485.45</v>
       </c>
@@ -7283,6 +7172,9 @@
         <f t="shared" si="0"/>
         <v>4652.9399999999987</v>
       </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
       <c r="C92">
         <v>1537.9</v>
       </c>
@@ -7319,6 +7211,9 @@
         <f t="shared" si="0"/>
         <v>4634.619999999999</v>
       </c>
+      <c r="B96">
+        <v>2.86</v>
+      </c>
       <c r="C96">
         <v>1556.22</v>
       </c>
@@ -7328,6 +7223,9 @@
         <f t="shared" si="0"/>
         <v>4620.99</v>
       </c>
+      <c r="B97">
+        <v>0.23</v>
+      </c>
       <c r="C97">
         <v>1569.85</v>
       </c>
@@ -7346,6 +7244,9 @@
         <f t="shared" si="0"/>
         <v>4604.4599999999991</v>
       </c>
+      <c r="B99">
+        <v>0.8</v>
+      </c>
       <c r="C99">
         <v>1586.38</v>
       </c>
@@ -7382,6 +7283,9 @@
         <f t="shared" si="0"/>
         <v>4578.7999999999993</v>
       </c>
+      <c r="B103">
+        <v>0.83</v>
+      </c>
       <c r="C103">
         <v>1612.04</v>
       </c>
@@ -7409,6 +7313,9 @@
         <f t="shared" si="0"/>
         <v>4562.619999999999</v>
       </c>
+      <c r="B106">
+        <v>5.72</v>
+      </c>
       <c r="C106">
         <v>1628.22</v>
       </c>
@@ -7427,6 +7334,9 @@
         <f t="shared" si="0"/>
         <v>4557.5199999999995</v>
       </c>
+      <c r="B108">
+        <v>0.74</v>
+      </c>
       <c r="C108">
         <v>1633.32</v>
       </c>
@@ -7445,6 +7355,9 @@
         <f t="shared" si="0"/>
         <v>4532.6399999999994</v>
       </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
       <c r="C110">
         <v>1658.2</v>
       </c>
@@ -7454,6 +7367,9 @@
         <f t="shared" si="0"/>
         <v>4530.2499999999991</v>
       </c>
+      <c r="B111">
+        <v>0.27</v>
+      </c>
       <c r="C111">
         <v>1660.59</v>
       </c>
@@ -7472,6 +7388,9 @@
         <f t="shared" si="0"/>
         <v>4527.1999999999989</v>
       </c>
+      <c r="B113">
+        <v>0.44</v>
+      </c>
       <c r="C113">
         <v>1663.64</v>
       </c>
@@ -7490,6 +7409,9 @@
         <f t="shared" si="0"/>
         <v>4518.0899999999992</v>
       </c>
+      <c r="B115">
+        <v>7.94</v>
+      </c>
       <c r="C115">
         <v>1672.75</v>
       </c>
@@ -7499,6 +7421,9 @@
         <f t="shared" si="0"/>
         <v>4513.74</v>
       </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
       <c r="C116">
         <v>1677.1</v>
       </c>
@@ -7526,6 +7451,9 @@
         <f t="shared" si="0"/>
         <v>4499.6399999999994</v>
       </c>
+      <c r="B119">
+        <v>0.16</v>
+      </c>
       <c r="C119">
         <v>1691.2</v>
       </c>
@@ -7562,6 +7490,9 @@
         <f t="shared" si="0"/>
         <v>4474.24</v>
       </c>
+      <c r="B123">
+        <v>0.13</v>
+      </c>
       <c r="C123">
         <v>1716.6</v>
       </c>
@@ -7571,6 +7502,9 @@
         <f t="shared" si="0"/>
         <v>4465.1899999999987</v>
       </c>
+      <c r="B124">
+        <v>0.27</v>
+      </c>
       <c r="C124">
         <v>1725.65</v>
       </c>
@@ -7580,6 +7514,9 @@
         <f t="shared" si="0"/>
         <v>4460.3599999999988</v>
       </c>
+      <c r="B125">
+        <v>2.39</v>
+      </c>
       <c r="C125">
         <v>1730.48</v>
       </c>
@@ -7598,6 +7535,9 @@
         <f t="shared" si="0"/>
         <v>4453.6399999999994</v>
       </c>
+      <c r="B127">
+        <v>0.41</v>
+      </c>
       <c r="C127">
         <v>1737.2</v>
       </c>
@@ -7625,6 +7565,9 @@
         <f t="shared" si="0"/>
         <v>4444.0399999999991</v>
       </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
       <c r="C130">
         <v>1746.8</v>
       </c>
@@ -7643,6 +7586,9 @@
         <f t="shared" si="0"/>
         <v>4405.2599999999993</v>
       </c>
+      <c r="B132">
+        <v>0.33</v>
+      </c>
       <c r="C132">
         <v>1785.58</v>
       </c>
@@ -7652,6 +7598,9 @@
         <f t="shared" si="0"/>
         <v>4401.079999999999</v>
       </c>
+      <c r="B133">
+        <v>0.41</v>
+      </c>
       <c r="C133">
         <v>1789.76</v>
       </c>
@@ -7679,6 +7628,9 @@
         <f t="shared" si="0"/>
         <v>4379.7299999999996</v>
       </c>
+      <c r="B136">
+        <v>3.48</v>
+      </c>
       <c r="C136">
         <v>1811.11</v>
       </c>
@@ -7688,6 +7640,9 @@
         <f t="shared" si="0"/>
         <v>4376.9399999999987</v>
       </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
       <c r="C137">
         <v>1813.9</v>
       </c>
@@ -7715,6 +7670,9 @@
         <f t="shared" si="0"/>
         <v>4366.9799999999996</v>
       </c>
+      <c r="B140">
+        <v>4.7300000000000004</v>
+      </c>
       <c r="C140">
         <v>1823.86</v>
       </c>
@@ -7724,6 +7682,9 @@
         <f t="shared" si="0"/>
         <v>4362.74</v>
       </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
       <c r="C141">
         <v>1828.1</v>
       </c>
@@ -7733,6 +7694,9 @@
         <f t="shared" si="0"/>
         <v>4357.0299999999988</v>
       </c>
+      <c r="B142">
+        <v>0.43</v>
+      </c>
       <c r="C142">
         <v>1833.81</v>
       </c>
@@ -7742,6 +7706,9 @@
         <f t="shared" si="0"/>
         <v>4353.6399999999994</v>
       </c>
+      <c r="B143">
+        <v>0.25</v>
+      </c>
       <c r="C143">
         <v>1837.2</v>
       </c>
@@ -7760,6 +7727,9 @@
         <f t="shared" si="0"/>
         <v>4344.1399999999994</v>
       </c>
+      <c r="B145">
+        <v>0.06</v>
+      </c>
       <c r="C145">
         <v>1846.7</v>
       </c>
@@ -7778,6 +7748,9 @@
         <f t="shared" si="0"/>
         <v>4321.1499999999996</v>
       </c>
+      <c r="B147">
+        <v>1.04</v>
+      </c>
       <c r="C147">
         <v>1869.69</v>
       </c>
@@ -7796,6 +7769,9 @@
         <f t="shared" si="0"/>
         <v>4304.6899999999987</v>
       </c>
+      <c r="B149">
+        <v>4.21</v>
+      </c>
       <c r="C149">
         <v>1886.15</v>
       </c>
@@ -7814,6 +7790,9 @@
         <f t="shared" si="0"/>
         <v>4297.0199999999995</v>
       </c>
+      <c r="B151">
+        <v>0.73</v>
+      </c>
       <c r="C151">
         <v>1893.82</v>
       </c>
@@ -7832,6 +7811,9 @@
         <f t="shared" si="0"/>
         <v>4289.9999999999991</v>
       </c>
+      <c r="B153">
+        <v>0.85</v>
+      </c>
       <c r="C153">
         <v>1900.84</v>
       </c>
@@ -7850,6 +7832,9 @@
         <f t="shared" si="0"/>
         <v>4275.4499999999989</v>
       </c>
+      <c r="B155">
+        <v>0.25</v>
+      </c>
       <c r="C155">
         <v>1915.39</v>
       </c>
@@ -7859,6 +7844,9 @@
         <f t="shared" si="0"/>
         <v>4258.74</v>
       </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
       <c r="C156">
         <v>1932.1</v>
       </c>
@@ -7868,6 +7856,9 @@
         <f t="shared" si="0"/>
         <v>4246.5299999999988</v>
       </c>
+      <c r="B157">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="C157">
         <v>1944.31</v>
       </c>
@@ -7877,6 +7868,9 @@
         <f t="shared" si="0"/>
         <v>4238.3399999999992</v>
       </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
       <c r="C158">
         <v>1952.5</v>
       </c>
@@ -7886,6 +7880,9 @@
         <f t="shared" si="0"/>
         <v>4226.119999999999</v>
       </c>
+      <c r="B159">
+        <v>0.37</v>
+      </c>
       <c r="C159">
         <v>1964.72</v>
       </c>
@@ -7895,6 +7892,9 @@
         <f t="shared" si="0"/>
         <v>4215.0399999999991</v>
       </c>
+      <c r="B160">
+        <v>0.22</v>
+      </c>
       <c r="C160">
         <v>1975.8</v>
       </c>
@@ -7904,6 +7904,9 @@
         <f t="shared" si="0"/>
         <v>4208.6399999999994</v>
       </c>
+      <c r="B161">
+        <v>0.36</v>
+      </c>
       <c r="C161">
         <v>1982.2</v>
       </c>
@@ -7922,6 +7925,9 @@
         <f t="shared" si="0"/>
         <v>4200.2799999999988</v>
       </c>
+      <c r="B163">
+        <v>0.9</v>
+      </c>
       <c r="C163">
         <v>1990.56</v>
       </c>
@@ -7958,6 +7964,9 @@
         <f t="shared" si="0"/>
         <v>4162.3799999999992</v>
       </c>
+      <c r="B167">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="C167">
         <v>2028.46</v>
       </c>
@@ -7994,6 +8003,9 @@
         <f t="shared" si="0"/>
         <v>4133.1399999999994</v>
       </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
       <c r="C171">
         <v>2057.6999999999998</v>
       </c>
@@ -8003,6 +8015,9 @@
         <f t="shared" si="0"/>
         <v>4131.4799999999996</v>
       </c>
+      <c r="B172">
+        <v>1.1100000000000001</v>
+      </c>
       <c r="C172">
         <v>2059.36</v>
       </c>
@@ -8012,6 +8027,9 @@
         <f t="shared" si="0"/>
         <v>4099.3399999999992</v>
       </c>
+      <c r="B173">
+        <v>0.18</v>
+      </c>
       <c r="C173">
         <v>2091.5</v>
       </c>
@@ -8021,6 +8039,9 @@
         <f t="shared" si="0"/>
         <v>4095.3399999999992</v>
       </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
       <c r="C174">
         <v>2095.5</v>
       </c>
@@ -8030,6 +8051,9 @@
         <f t="shared" si="0"/>
         <v>4091.559999999999</v>
       </c>
+      <c r="B175">
+        <v>1.37</v>
+      </c>
       <c r="C175">
         <v>2099.2800000000002</v>
       </c>
@@ -8048,6 +8072,9 @@
         <f t="shared" si="0"/>
         <v>4079.2399999999993</v>
       </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
       <c r="C177">
         <v>2111.6</v>
       </c>
@@ -8057,6 +8084,9 @@
         <f t="shared" si="0"/>
         <v>4064.4899999999993</v>
       </c>
+      <c r="B178">
+        <v>2.83</v>
+      </c>
       <c r="C178">
         <v>2126.35</v>
       </c>
@@ -8066,6 +8096,9 @@
         <f t="shared" si="0"/>
         <v>4060.6399999999994</v>
       </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
       <c r="C179">
         <v>2130.1999999999998</v>
       </c>
@@ -8075,6 +8108,9 @@
         <f t="shared" si="0"/>
         <v>4037.9399999999991</v>
       </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
       <c r="C180">
         <v>2152.9</v>
       </c>
@@ -8093,6 +8129,9 @@
         <f t="shared" si="0"/>
         <v>4033.3599999999992</v>
       </c>
+      <c r="B182">
+        <v>0.53</v>
+      </c>
       <c r="C182">
         <v>2157.48</v>
       </c>
@@ -8102,6 +8141,9 @@
         <f t="shared" si="0"/>
         <v>4026.0199999999991</v>
       </c>
+      <c r="B183">
+        <v>3.32</v>
+      </c>
       <c r="C183">
         <v>2164.8200000000002</v>
       </c>
@@ -8120,6 +8162,9 @@
         <f t="shared" si="0"/>
         <v>4020.9699999999993</v>
       </c>
+      <c r="B185">
+        <v>0.47</v>
+      </c>
       <c r="C185">
         <v>2169.87</v>
       </c>
@@ -8129,6 +8174,9 @@
         <f t="shared" si="0"/>
         <v>4014.0899999999992</v>
       </c>
+      <c r="B186">
+        <v>6.44</v>
+      </c>
       <c r="C186">
         <v>2176.75</v>
       </c>
@@ -8138,6 +8186,9 @@
         <f t="shared" si="0"/>
         <v>3981.7899999999991</v>
       </c>
+      <c r="B187">
+        <v>1.28</v>
+      </c>
       <c r="C187">
         <v>2209.0500000000002</v>
       </c>
@@ -8156,6 +8207,9 @@
         <f t="shared" si="0"/>
         <v>3959.3799999999992</v>
       </c>
+      <c r="B189">
+        <v>0.35</v>
+      </c>
       <c r="C189">
         <v>2231.46</v>
       </c>
@@ -8174,6 +8228,9 @@
         <f t="shared" si="0"/>
         <v>3955.1199999999994</v>
       </c>
+      <c r="B191">
+        <v>1.42</v>
+      </c>
       <c r="C191">
         <v>2235.7199999999998</v>
       </c>
@@ -8183,20 +8240,26 @@
         <f t="shared" si="0"/>
         <v>3951.7399999999993</v>
       </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
       <c r="C192">
         <v>2239.1</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193">
         <f t="shared" si="0"/>
         <v>3942.7599999999993</v>
+      </c>
+      <c r="B193">
+        <v>1.65</v>
       </c>
       <c r="C193">
         <v>2248.08</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194">
         <f t="shared" si="0"/>
         <v>3937.4699999999993</v>
@@ -8205,34 +8268,43 @@
         <v>2253.37</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195">
         <f t="shared" si="0"/>
         <v>3933.2399999999993</v>
+      </c>
+      <c r="B195">
+        <v>0.11</v>
       </c>
       <c r="C195">
         <v>2257.6</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196">
         <f t="shared" si="0"/>
         <v>3927.9399999999991</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
       </c>
       <c r="C196">
         <v>2262.9</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197">
         <f t="shared" si="0"/>
         <v>3924.5399999999991</v>
+      </c>
+      <c r="B197">
+        <v>0.23</v>
       </c>
       <c r="C197">
         <v>2266.3000000000002</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198">
         <f t="shared" si="0"/>
         <v>3921.1499999999992</v>
@@ -8241,1404 +8313,1494 @@
         <v>2269.69</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199">
         <f t="shared" si="0"/>
         <v>3907.8699999999994</v>
+      </c>
+      <c r="B199">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C199">
         <v>2282.9699999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200">
         <f t="shared" si="0"/>
         <v>3898.2499999999991</v>
+      </c>
+      <c r="B200">
+        <v>1.01</v>
       </c>
       <c r="C200">
         <v>2292.59</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201">
         <f t="shared" si="0"/>
         <v>3886.9299999999994</v>
+      </c>
+      <c r="B201">
+        <v>2.68</v>
       </c>
       <c r="C201">
         <v>2303.91</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202">
         <f t="shared" si="0"/>
         <v>3879.0399999999991</v>
+      </c>
+      <c r="B202">
+        <v>0</v>
       </c>
       <c r="C202">
         <v>2311.8000000000002</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203">
+        <f t="shared" ref="A203" si="1">$E$1-C203</f>
+        <v>3875.8599999999992</v>
+      </c>
+      <c r="B203">
+        <v>0.33</v>
+      </c>
+      <c r="C203">
+        <v>2314.98</v>
+      </c>
+      <c r="D203" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204">
         <f t="shared" si="0"/>
         <v>3866.1699999999992</v>
       </c>
-      <c r="C203">
+      <c r="C204">
         <v>2324.67</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A204">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205">
         <f t="shared" si="0"/>
         <v>3865.2399999999993</v>
       </c>
-      <c r="C204">
+      <c r="B205">
+        <v>2.08</v>
+      </c>
+      <c r="C205">
         <v>2325.6</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A205">
-        <f t="shared" si="0"/>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <f t="shared" ref="A206" si="2">$E$1-C206</f>
         <v>3850.5099999999993</v>
       </c>
-      <c r="C205">
+      <c r="C206">
         <v>2340.33</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <f t="shared" si="0"/>
+        <v>3841.1399999999994</v>
+      </c>
+      <c r="B207">
+        <v>0.17</v>
+      </c>
+      <c r="C207">
+        <v>2349.6999999999998</v>
+      </c>
+      <c r="D207" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
         <f t="shared" si="0"/>
         <v>3831.0999999999995</v>
       </c>
-      <c r="C206">
+      <c r="B208">
+        <v>0.4</v>
+      </c>
+      <c r="C208">
         <v>2359.7399999999998</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207">
-        <f t="shared" si="0"/>
-        <v>3824.4399999999991</v>
-      </c>
-      <c r="C207">
-        <v>2366.4</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208">
-        <f t="shared" si="0"/>
-        <v>3823.4399999999991</v>
-      </c>
-      <c r="C208">
-        <v>2367.4</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209">
         <f t="shared" si="0"/>
-        <v>3821.7899999999991</v>
+        <v>3824.4399999999991</v>
       </c>
       <c r="C209">
-        <v>2369.0500000000002</v>
+        <v>2366.4</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210">
         <f t="shared" si="0"/>
-        <v>3817.6399999999994</v>
+        <v>3823.4399999999991</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
       </c>
       <c r="C210">
-        <v>2373.1999999999998</v>
+        <v>2367.4</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211">
         <f t="shared" si="0"/>
-        <v>3806.7499999999991</v>
+        <v>3821.7899999999991</v>
+      </c>
+      <c r="B211">
+        <v>2.1800000000000002</v>
       </c>
       <c r="C211">
-        <v>2384.09</v>
+        <v>2369.0500000000002</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212">
         <f t="shared" si="0"/>
-        <v>3798.1299999999992</v>
+        <v>3817.6399999999994</v>
+      </c>
+      <c r="B212">
+        <v>0.22</v>
       </c>
       <c r="C212">
-        <v>2392.71</v>
+        <v>2373.1999999999998</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213">
         <f t="shared" si="0"/>
-        <v>3777.5899999999992</v>
+        <v>3806.7499999999991</v>
+      </c>
+      <c r="B213">
+        <v>1.57</v>
       </c>
       <c r="C213">
-        <v>2413.25</v>
+        <v>2384.09</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214">
         <f t="shared" si="0"/>
-        <v>3773.559999999999</v>
+        <v>3798.1299999999992</v>
+      </c>
+      <c r="B214">
+        <v>3.02</v>
       </c>
       <c r="C214">
-        <v>2417.2800000000002</v>
+        <v>2392.71</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215">
         <f t="shared" si="0"/>
-        <v>3772.7399999999993</v>
+        <v>3777.5899999999992</v>
       </c>
       <c r="C215">
-        <v>2418.1</v>
+        <v>2413.25</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216">
         <f t="shared" si="0"/>
-        <v>3762.7999999999993</v>
+        <v>3773.3599999999992</v>
+      </c>
+      <c r="B216">
+        <v>1.2</v>
       </c>
       <c r="C216">
-        <v>2428.04</v>
+        <v>2417.48</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217">
         <f t="shared" si="0"/>
-        <v>3761.0499999999993</v>
+        <v>3772.7399999999993</v>
       </c>
       <c r="C217">
-        <v>2429.79</v>
+        <v>2418.1</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218">
         <f t="shared" si="0"/>
-        <v>3759.7399999999993</v>
+        <v>3762.7999999999993</v>
+      </c>
+      <c r="B218">
+        <v>1.0900000000000001</v>
       </c>
       <c r="C218">
-        <v>2431.1</v>
+        <v>2428.04</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219">
         <f t="shared" si="0"/>
-        <v>3757.6399999999994</v>
+        <v>3761.0499999999993</v>
       </c>
       <c r="C219">
-        <v>2433.1999999999998</v>
+        <v>2429.79</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220">
         <f t="shared" si="0"/>
-        <v>3757.2099999999991</v>
+        <v>3759.7399999999993</v>
+      </c>
+      <c r="B220">
+        <v>0</v>
       </c>
       <c r="C220">
-        <v>2433.63</v>
+        <v>2431.1</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221">
         <f t="shared" si="0"/>
-        <v>3743.1399999999994</v>
+        <v>3757.6399999999994</v>
       </c>
       <c r="C221">
-        <v>2447.6999999999998</v>
+        <v>2433.1999999999998</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222">
         <f t="shared" si="0"/>
-        <v>3740.4399999999991</v>
+        <v>3757.2099999999991</v>
+      </c>
+      <c r="B222">
+        <v>1.33</v>
       </c>
       <c r="C222">
-        <v>2450.4</v>
+        <v>2433.63</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223">
         <f t="shared" si="0"/>
-        <v>3740.2799999999993</v>
+        <v>3743.1399999999994</v>
+      </c>
+      <c r="B223">
+        <v>0</v>
       </c>
       <c r="C223">
-        <v>2450.56</v>
+        <v>2447.6999999999998</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224">
         <f t="shared" si="0"/>
-        <v>3730.7399999999993</v>
+        <v>3740.4399999999991</v>
       </c>
       <c r="C224">
-        <v>2460.1</v>
+        <v>2450.4</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225">
         <f t="shared" si="0"/>
-        <v>3715.8399999999992</v>
+        <v>3740.2799999999993</v>
       </c>
       <c r="B225">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="C225">
-        <v>2475</v>
+        <v>2450.56</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226">
         <f t="shared" si="0"/>
-        <v>3709.3799999999992</v>
+        <v>3730.7399999999993</v>
       </c>
       <c r="B226">
-        <v>1.29</v>
+        <v>0.54</v>
       </c>
       <c r="C226">
-        <v>2481.46</v>
+        <v>2460.1</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227">
         <f t="shared" si="0"/>
-        <v>3705.2399999999993</v>
+        <v>3715.8399999999992</v>
       </c>
       <c r="B227">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="C227">
-        <v>2485.6</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228">
         <f t="shared" si="0"/>
-        <v>3697.8599999999992</v>
+        <v>3709.3799999999992</v>
       </c>
       <c r="B228">
-        <v>0.88</v>
+        <v>1.29</v>
       </c>
       <c r="C228">
-        <v>2492.98</v>
+        <v>2481.46</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229">
         <f t="shared" si="0"/>
-        <v>3696.9399999999991</v>
+        <v>3705.2399999999993</v>
+      </c>
+      <c r="B229">
+        <v>0.39</v>
       </c>
       <c r="C229">
-        <v>2493.9</v>
+        <v>2485.6</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230">
         <f t="shared" si="0"/>
-        <v>3687.5899999999992</v>
+        <v>3697.8599999999992</v>
       </c>
       <c r="B230">
-        <v>2.39</v>
+        <v>0.88</v>
       </c>
       <c r="C230">
-        <v>2503.25</v>
+        <v>2492.98</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231">
         <f t="shared" si="0"/>
-        <v>3674.2399999999993</v>
+        <v>3696.9399999999991</v>
       </c>
       <c r="C231">
-        <v>2516.6</v>
+        <v>2493.9</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232">
         <f t="shared" si="0"/>
-        <v>3673.1699999999992</v>
+        <v>3687.5899999999992</v>
       </c>
       <c r="B232">
-        <v>1.1000000000000001</v>
+        <v>2.39</v>
       </c>
       <c r="C232">
-        <v>2517.67</v>
+        <v>2503.25</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233">
         <f t="shared" si="0"/>
-        <v>3668.3399999999992</v>
-      </c>
-      <c r="B233">
-        <v>3.9</v>
+        <v>3674.2399999999993</v>
       </c>
       <c r="C233">
-        <v>2522.5</v>
+        <v>2516.6</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234">
         <f t="shared" si="0"/>
-        <v>3667.7999999999993</v>
+        <v>3673.1699999999992</v>
+      </c>
+      <c r="B234">
+        <v>1.1000000000000001</v>
       </c>
       <c r="C234">
-        <v>2523.04</v>
+        <v>2517.67</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235">
         <f t="shared" si="0"/>
-        <v>3660.7399999999993</v>
+        <v>3668.3399999999992</v>
       </c>
       <c r="B235">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="C235">
-        <v>2530.1</v>
+        <v>2522.5</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236">
         <f t="shared" si="0"/>
-        <v>3655.6799999999994</v>
-      </c>
-      <c r="B236">
-        <v>2.11</v>
+        <v>3667.7999999999993</v>
       </c>
       <c r="C236">
-        <v>2535.16</v>
+        <v>2523.04</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237">
         <f t="shared" si="0"/>
-        <v>3654.6899999999991</v>
+        <v>3660.7399999999993</v>
+      </c>
+      <c r="B237">
+        <v>0</v>
       </c>
       <c r="C237">
-        <v>2536.15</v>
+        <v>2530.1</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238">
         <f t="shared" si="0"/>
-        <v>3643.2399999999993</v>
+        <v>3655.6799999999994</v>
       </c>
       <c r="B238">
-        <v>0</v>
+        <v>2.11</v>
       </c>
       <c r="C238">
-        <v>2547.6</v>
+        <v>2535.16</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239">
         <f t="shared" si="0"/>
-        <v>3640.5399999999991</v>
-      </c>
-      <c r="B239">
-        <v>0</v>
+        <v>3654.6899999999991</v>
       </c>
       <c r="C239">
-        <v>2550.3000000000002</v>
+        <v>2536.15</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240">
         <f t="shared" si="0"/>
-        <v>3638.0399999999991</v>
+        <v>3643.2399999999993</v>
       </c>
       <c r="B240">
         <v>0</v>
       </c>
       <c r="C240">
-        <v>2552.8000000000002</v>
+        <v>2547.6</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
         <f t="shared" si="0"/>
-        <v>3631.0099999999993</v>
+        <v>3640.5399999999991</v>
+      </c>
+      <c r="B241">
+        <v>0</v>
       </c>
       <c r="C241">
-        <v>2559.83</v>
+        <v>2550.3000000000002</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
         <f t="shared" si="0"/>
-        <v>3622.9399999999991</v>
+        <v>3638.0399999999991</v>
       </c>
       <c r="B242">
         <v>0</v>
       </c>
       <c r="C242">
-        <v>2567.9</v>
+        <v>2552.8000000000002</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
         <f t="shared" si="0"/>
-        <v>3616.8399999999992</v>
-      </c>
-      <c r="B243">
-        <v>0</v>
+        <v>3631.0099999999993</v>
       </c>
       <c r="C243">
-        <v>2574</v>
+        <v>2559.83</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
         <f t="shared" si="0"/>
-        <v>3599.5999999999995</v>
+        <v>3622.9399999999991</v>
+      </c>
+      <c r="B244">
+        <v>0</v>
       </c>
       <c r="C244">
-        <v>2591.2399999999998</v>
+        <v>2567.9</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245">
         <f t="shared" si="0"/>
-        <v>3597.4499999999994</v>
+        <v>3616.8399999999992</v>
       </c>
       <c r="B245">
-        <v>0.78</v>
+        <v>0</v>
       </c>
       <c r="C245">
-        <v>2593.39</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
         <f t="shared" si="0"/>
-        <v>3593.0399999999991</v>
-      </c>
-      <c r="B246">
-        <v>0</v>
+        <v>3599.5999999999995</v>
       </c>
       <c r="C246">
-        <v>2597.8000000000002</v>
+        <v>2591.2399999999998</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
         <f t="shared" si="0"/>
-        <v>3582.309999999999</v>
+        <v>3597.4499999999994</v>
       </c>
       <c r="B247">
-        <v>0.59</v>
+        <v>0.78</v>
       </c>
       <c r="C247">
-        <v>2608.5300000000002</v>
+        <v>2593.39</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248">
         <f t="shared" si="0"/>
-        <v>3579.6399999999994</v>
+        <v>3593.0399999999991</v>
+      </c>
+      <c r="B248">
+        <v>0</v>
       </c>
       <c r="C248">
-        <v>2611.1999999999998</v>
+        <v>2597.8000000000002</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249">
         <f t="shared" si="0"/>
-        <v>3578.1399999999994</v>
+        <v>3582.309999999999</v>
       </c>
       <c r="B249">
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="C249">
-        <v>2612.6999999999998</v>
+        <v>2608.5300000000002</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250">
         <f t="shared" si="0"/>
-        <v>3575.0499999999993</v>
-      </c>
-      <c r="B250">
-        <v>0</v>
+        <v>3579.6399999999994</v>
       </c>
       <c r="C250">
-        <v>2615.79</v>
+        <v>2611.1999999999998</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251">
         <f t="shared" si="0"/>
-        <v>3567.809999999999</v>
+        <v>3578.1399999999994</v>
       </c>
       <c r="B251">
-        <v>1.61</v>
+        <v>0</v>
       </c>
       <c r="C251">
-        <v>2623.03</v>
+        <v>2612.6999999999998</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252">
         <f t="shared" si="0"/>
-        <v>3561.6699999999992</v>
+        <v>3575.0499999999993</v>
       </c>
       <c r="B252">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="C252">
-        <v>2629.17</v>
+        <v>2615.79</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253">
         <f t="shared" si="0"/>
-        <v>3541.4199999999992</v>
+        <v>3567.809999999999</v>
+      </c>
+      <c r="B253">
+        <v>1.61</v>
       </c>
       <c r="C253">
-        <v>2649.42</v>
+        <v>2623.03</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254">
         <f t="shared" si="0"/>
-        <v>3535.3699999999994</v>
+        <v>3561.6699999999992</v>
+      </c>
+      <c r="B254">
+        <v>1.04</v>
       </c>
       <c r="C254">
-        <v>2655.47</v>
+        <v>2629.17</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255">
         <f t="shared" si="0"/>
-        <v>3535.0399999999991</v>
+        <v>3541.4199999999992</v>
       </c>
       <c r="C255">
-        <v>2655.8</v>
+        <v>2649.42</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256">
         <f t="shared" si="0"/>
-        <v>3534.579999999999</v>
-      </c>
-      <c r="B256">
-        <v>0.62</v>
+        <v>3535.3699999999994</v>
       </c>
       <c r="C256">
-        <v>2656.26</v>
+        <v>2655.47</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
         <f t="shared" si="0"/>
-        <v>3522.4399999999991</v>
-      </c>
-      <c r="B257">
-        <v>0.56999999999999995</v>
+        <v>3535.0399999999991</v>
       </c>
       <c r="C257">
-        <v>2668.4</v>
+        <v>2655.8</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
         <f t="shared" si="0"/>
-        <v>3503.0699999999993</v>
+        <v>3534.579999999999</v>
       </c>
       <c r="B258">
-        <v>1.01</v>
+        <v>0.62</v>
       </c>
       <c r="C258">
-        <v>2687.77</v>
+        <v>2656.26</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
-        <f t="shared" ref="A259:A332" si="2">$E$1-C259</f>
-        <v>3493.8399999999992</v>
+        <f t="shared" si="0"/>
+        <v>3522.4399999999991</v>
+      </c>
+      <c r="B259">
+        <v>0.56999999999999995</v>
       </c>
       <c r="C259">
-        <v>2697</v>
+        <v>2668.4</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
-        <f t="shared" si="2"/>
-        <v>3491.6799999999994</v>
+        <f t="shared" si="0"/>
+        <v>3503.0699999999993</v>
       </c>
       <c r="B260">
-        <v>1.61</v>
+        <v>1.01</v>
       </c>
       <c r="C260">
-        <v>2699.16</v>
+        <v>2687.77</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261">
-        <f t="shared" si="2"/>
-        <v>3484.2499999999991</v>
+        <f t="shared" ref="A261:A333" si="3">$E$1-C261</f>
+        <v>3493.8399999999992</v>
       </c>
       <c r="C261">
-        <v>2706.59</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
-        <f t="shared" si="2"/>
-        <v>3482.7299999999991</v>
+        <f t="shared" si="3"/>
+        <v>3491.6799999999994</v>
       </c>
       <c r="B262">
-        <v>1.65</v>
+        <v>1.61</v>
       </c>
       <c r="C262">
-        <v>2708.11</v>
+        <v>2699.16</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
-        <f t="shared" si="2"/>
-        <v>3475.329999999999</v>
-      </c>
-      <c r="B263">
-        <v>1.89</v>
+        <f t="shared" si="3"/>
+        <v>3484.2499999999991</v>
       </c>
       <c r="C263">
-        <v>2715.51</v>
+        <v>2706.59</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
-        <f t="shared" si="2"/>
-        <v>3468.0999999999995</v>
+        <f t="shared" si="3"/>
+        <v>3482.7299999999991</v>
       </c>
       <c r="B264">
-        <v>1.4</v>
+        <v>1.65</v>
       </c>
       <c r="C264">
-        <v>2722.74</v>
+        <v>2708.11</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
-        <f t="shared" si="2"/>
-        <v>3467.579999999999</v>
+        <f t="shared" si="3"/>
+        <v>3475.329999999999</v>
+      </c>
+      <c r="B265">
+        <v>1.89</v>
       </c>
       <c r="C265">
-        <v>2723.26</v>
+        <v>2715.51</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
-        <f t="shared" si="2"/>
-        <v>3452.8399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3468.0999999999995</v>
+      </c>
+      <c r="B266">
+        <v>1.4</v>
       </c>
       <c r="C266">
-        <v>2738</v>
+        <v>2722.74</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267">
-        <f t="shared" si="2"/>
-        <v>3449.4399999999991</v>
-      </c>
-      <c r="B267">
-        <v>0.79</v>
+        <f t="shared" si="3"/>
+        <v>3467.579999999999</v>
       </c>
       <c r="C267">
-        <v>2741.4</v>
+        <v>2723.26</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268">
-        <f t="shared" si="2"/>
-        <v>3446.8399999999992</v>
-      </c>
-      <c r="B268">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3452.8399999999992</v>
       </c>
       <c r="C268">
-        <v>2744</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
-        <f t="shared" si="2"/>
-        <v>3425.6399999999994</v>
+        <f t="shared" si="3"/>
+        <v>3449.4399999999991</v>
       </c>
       <c r="B269">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="C269">
-        <v>2765.2</v>
+        <v>2741.4</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270">
-        <f t="shared" si="2"/>
-        <v>3422.2799999999993</v>
+        <f t="shared" si="3"/>
+        <v>3446.8399999999992</v>
       </c>
       <c r="B270">
-        <v>1.58</v>
+        <v>0</v>
       </c>
       <c r="C270">
-        <v>2768.56</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271">
-        <f t="shared" si="2"/>
-        <v>3420.8399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3425.6399999999994</v>
       </c>
       <c r="B271">
-        <v>0.68</v>
+        <v>0</v>
       </c>
       <c r="C271">
-        <v>2770</v>
+        <v>2765.2</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
-        <f t="shared" si="2"/>
-        <v>3417.9399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3422.2799999999993</v>
       </c>
       <c r="B272">
-        <v>0.5</v>
+        <v>1.58</v>
       </c>
       <c r="C272">
-        <v>2772.9</v>
+        <v>2768.56</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273">
-        <f t="shared" si="2"/>
-        <v>3408.5199999999991</v>
+        <f t="shared" si="3"/>
+        <v>3420.8399999999992</v>
       </c>
       <c r="B273">
-        <v>1.91</v>
+        <v>0.68</v>
       </c>
       <c r="C273">
-        <v>2782.32</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274">
-        <f t="shared" si="2"/>
-        <v>3407.5099999999993</v>
+        <f t="shared" si="3"/>
+        <v>3417.9399999999991</v>
+      </c>
+      <c r="B274">
+        <v>0.5</v>
       </c>
       <c r="C274">
-        <v>2783.33</v>
+        <v>2772.9</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275">
-        <f t="shared" si="2"/>
-        <v>3385.8799999999992</v>
+        <f t="shared" si="3"/>
+        <v>3408.5199999999991</v>
       </c>
       <c r="B275">
-        <v>0.4</v>
+        <v>1.91</v>
       </c>
       <c r="C275">
-        <v>2804.96</v>
+        <v>2782.32</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276">
-        <f t="shared" si="2"/>
-        <v>3377.5299999999993</v>
-      </c>
-      <c r="B276">
-        <v>0.48</v>
+        <f t="shared" si="3"/>
+        <v>3407.5099999999993</v>
       </c>
       <c r="C276">
-        <v>2813.31</v>
+        <v>2783.33</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277">
-        <f t="shared" si="2"/>
-        <v>3375.0399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3385.8799999999992</v>
       </c>
       <c r="B277">
-        <v>1.19</v>
+        <v>0.4</v>
       </c>
       <c r="C277">
-        <v>2815.8</v>
+        <v>2804.96</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278">
-        <f t="shared" si="2"/>
-        <v>3373.5399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3377.5299999999993</v>
+      </c>
+      <c r="B278">
+        <v>0.48</v>
       </c>
       <c r="C278">
-        <v>2817.3</v>
+        <v>2813.31</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279">
-        <f t="shared" si="2"/>
-        <v>3357.9899999999993</v>
+        <f t="shared" si="3"/>
+        <v>3375.0399999999991</v>
       </c>
       <c r="B279">
-        <v>0</v>
+        <v>1.19</v>
       </c>
       <c r="C279">
-        <v>2832.85</v>
+        <v>2815.8</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280">
-        <f t="shared" si="2"/>
-        <v>3356.9299999999994</v>
-      </c>
-      <c r="B280">
-        <v>1.72</v>
+        <f t="shared" si="3"/>
+        <v>3373.5399999999991</v>
       </c>
       <c r="C280">
-        <v>2833.91</v>
+        <v>2817.3</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281">
-        <f t="shared" si="2"/>
-        <v>3353.1099999999992</v>
+        <f t="shared" si="3"/>
+        <v>3357.9899999999993</v>
+      </c>
+      <c r="B281">
+        <v>0</v>
       </c>
       <c r="C281">
-        <v>2837.73</v>
+        <v>2832.85</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282">
-        <f t="shared" si="2"/>
-        <v>3351.4399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3356.9299999999994</v>
       </c>
       <c r="B282">
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="C282">
-        <v>2839.4</v>
+        <v>2833.91</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283">
-        <f t="shared" si="2"/>
-        <v>3347.5399999999991</v>
-      </c>
-      <c r="B283">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3353.1099999999992</v>
       </c>
       <c r="C283">
-        <v>2843.3</v>
+        <v>2837.73</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284">
-        <f t="shared" si="2"/>
-        <v>3344.4299999999994</v>
+        <f t="shared" si="3"/>
+        <v>3351.4399999999991</v>
       </c>
       <c r="B284">
-        <v>2.0099999999999998</v>
+        <v>0</v>
       </c>
       <c r="C284">
-        <v>2846.41</v>
+        <v>2839.4</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285">
-        <f t="shared" si="2"/>
-        <v>3334.8399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3347.5399999999991</v>
       </c>
       <c r="B285">
         <v>0</v>
       </c>
       <c r="C285">
-        <v>2856</v>
+        <v>2843.3</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286">
-        <f t="shared" si="2"/>
-        <v>3316.7499999999991</v>
+        <f t="shared" si="3"/>
+        <v>3344.4299999999994</v>
+      </c>
+      <c r="B286">
+        <v>2.0099999999999998</v>
       </c>
       <c r="C286">
-        <v>2874.09</v>
+        <v>2846.41</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287">
-        <f t="shared" si="2"/>
-        <v>3309.6399999999994</v>
+        <f t="shared" si="3"/>
+        <v>3334.8399999999992</v>
+      </c>
+      <c r="B287">
+        <v>0</v>
       </c>
       <c r="C287">
-        <v>2881.2</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288">
-        <f t="shared" si="2"/>
-        <v>3306.7299999999991</v>
-      </c>
-      <c r="B288">
-        <v>1.03</v>
+        <f t="shared" si="3"/>
+        <v>3316.7499999999991</v>
       </c>
       <c r="C288">
-        <v>2884.11</v>
+        <v>2874.09</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289">
-        <f t="shared" si="2"/>
-        <v>3292.1399999999994</v>
+        <f t="shared" si="3"/>
+        <v>3309.6399999999994</v>
       </c>
       <c r="C289">
-        <v>2898.7</v>
+        <v>2881.2</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290">
-        <f t="shared" si="2"/>
-        <v>3280.5399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3306.7299999999991</v>
       </c>
       <c r="B290">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="C290">
-        <v>2910.3</v>
+        <v>2884.11</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291">
-        <f t="shared" si="2"/>
-        <v>3275.7199999999993</v>
-      </c>
-      <c r="B291">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3292.1399999999994</v>
       </c>
       <c r="C291">
-        <v>2915.12</v>
+        <v>2898.7</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292">
-        <f t="shared" si="2"/>
-        <v>3260.9499999999994</v>
+        <f t="shared" si="3"/>
+        <v>3280.5399999999991</v>
+      </c>
+      <c r="B292">
+        <v>0</v>
       </c>
       <c r="C292">
-        <v>2929.89</v>
+        <v>2910.3</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293">
-        <f t="shared" si="2"/>
-        <v>3258.2799999999993</v>
+        <f t="shared" si="3"/>
+        <v>3275.7199999999993</v>
+      </c>
+      <c r="B293">
+        <v>0</v>
       </c>
       <c r="C293">
-        <v>2932.56</v>
+        <v>2915.12</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294">
-        <f t="shared" si="2"/>
-        <v>3245.2399999999993</v>
-      </c>
-      <c r="B294">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3260.9499999999994</v>
       </c>
       <c r="C294">
-        <v>2945.6</v>
+        <v>2929.89</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295">
-        <f t="shared" si="2"/>
-        <v>3236.2399999999993</v>
-      </c>
-      <c r="B295">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3258.2799999999993</v>
       </c>
       <c r="C295">
-        <v>2954.6</v>
+        <v>2932.56</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296">
-        <f t="shared" si="2"/>
-        <v>3224.1399999999994</v>
+        <f t="shared" si="3"/>
+        <v>3245.2399999999993</v>
       </c>
       <c r="B296">
         <v>0</v>
       </c>
       <c r="C296">
-        <v>2966.7</v>
+        <v>2945.6</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297">
-        <f t="shared" si="2"/>
-        <v>3213.059999999999</v>
+        <f t="shared" si="3"/>
+        <v>3236.2399999999993</v>
+      </c>
+      <c r="B297">
+        <v>0</v>
       </c>
       <c r="C297">
-        <v>2977.78</v>
+        <v>2954.6</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298">
-        <f t="shared" si="2"/>
-        <v>3211.7599999999993</v>
+        <f t="shared" si="3"/>
+        <v>3224.1399999999994</v>
       </c>
       <c r="B298">
-        <v>2.42</v>
+        <v>0</v>
       </c>
       <c r="C298">
-        <v>2979.08</v>
+        <v>2966.7</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299">
-        <f t="shared" si="2"/>
-        <v>3179.9399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3213.059999999999</v>
       </c>
       <c r="C299">
-        <v>3010.9</v>
+        <v>2977.78</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300">
-        <f t="shared" si="2"/>
-        <v>3175.5399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3211.7599999999993</v>
       </c>
       <c r="B300">
-        <v>0</v>
+        <v>2.42</v>
       </c>
       <c r="C300">
-        <v>3015.3</v>
+        <v>2979.08</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301">
-        <f t="shared" si="2"/>
-        <v>3159.8399999999992</v>
-      </c>
-      <c r="B301">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3179.9399999999991</v>
       </c>
       <c r="C301">
-        <v>3031</v>
+        <v>3010.9</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302">
-        <f t="shared" si="2"/>
-        <v>3148.3399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3175.5399999999991</v>
       </c>
       <c r="B302">
         <v>0</v>
       </c>
       <c r="C302">
-        <v>3042.5</v>
+        <v>3015.3</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303">
-        <f t="shared" si="2"/>
-        <v>3136.3399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3159.8399999999992</v>
       </c>
       <c r="B303">
         <v>0</v>
       </c>
       <c r="C303">
-        <v>3054.5</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304">
-        <f t="shared" si="2"/>
-        <v>3119.8399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3148.3399999999992</v>
       </c>
       <c r="B304">
         <v>0</v>
       </c>
       <c r="C304">
-        <v>3071</v>
+        <v>3042.5</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305">
-        <f t="shared" si="2"/>
-        <v>3112.1399999999994</v>
+        <f t="shared" si="3"/>
+        <v>3136.3399999999992</v>
       </c>
       <c r="B305">
         <v>0</v>
       </c>
       <c r="C305">
-        <v>3078.7</v>
+        <v>3054.5</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306">
-        <f t="shared" si="2"/>
-        <v>3106.9399999999991</v>
+        <f t="shared" si="3"/>
+        <v>3119.8399999999992</v>
       </c>
       <c r="B306">
         <v>0</v>
       </c>
       <c r="C306">
-        <v>3083.9</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307">
-        <f t="shared" si="2"/>
-        <v>3094.3399999999992</v>
+        <f t="shared" si="3"/>
+        <v>3112.1399999999994</v>
+      </c>
+      <c r="B307">
+        <v>0</v>
       </c>
       <c r="C307">
-        <v>3096.5</v>
+        <v>3078.7</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308">
-        <f t="shared" si="2"/>
-        <v>3093.2699999999991</v>
+        <f t="shared" si="3"/>
+        <v>3106.9399999999991</v>
       </c>
       <c r="B308">
-        <v>2.04</v>
+        <v>0</v>
       </c>
       <c r="C308">
-        <v>3097.57</v>
+        <v>3083.9</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309">
-        <f t="shared" si="2"/>
-        <v>3034.059999999999</v>
+        <f t="shared" si="3"/>
+        <v>3094.3399999999992</v>
       </c>
       <c r="C309">
-        <v>3156.78</v>
+        <v>3096.5</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310">
-        <f t="shared" si="2"/>
-        <v>3029.5899999999992</v>
+        <f t="shared" si="3"/>
+        <v>3093.2699999999991</v>
+      </c>
+      <c r="B310">
+        <v>2.04</v>
       </c>
       <c r="C310">
-        <v>3161.25</v>
+        <v>3097.57</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311">
-        <f t="shared" si="2"/>
-        <v>2980.0999999999995</v>
-      </c>
-      <c r="B311">
-        <v>1.02</v>
+        <f t="shared" si="3"/>
+        <v>3034.059999999999</v>
       </c>
       <c r="C311">
-        <v>3210.74</v>
+        <v>3156.78</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312">
-        <f t="shared" si="2"/>
-        <v>2900.4999999999991</v>
+        <f t="shared" si="3"/>
+        <v>3029.5899999999992</v>
       </c>
       <c r="C312">
-        <v>3290.34</v>
+        <v>3161.25</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313">
-        <f t="shared" si="2"/>
-        <v>2898.3599999999992</v>
+        <f t="shared" si="3"/>
+        <v>2980.0999999999995</v>
+      </c>
+      <c r="B313">
+        <v>1.02</v>
       </c>
       <c r="C313">
-        <v>3292.48</v>
+        <v>3210.74</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314">
-        <f t="shared" si="2"/>
-        <v>2841.4699999999993</v>
+        <f t="shared" si="3"/>
+        <v>2900.4999999999991</v>
       </c>
       <c r="C314">
-        <v>3349.37</v>
+        <v>3290.34</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315">
-        <f t="shared" si="2"/>
-        <v>2767.0499999999993</v>
+        <f t="shared" si="3"/>
+        <v>2898.3599999999992</v>
       </c>
       <c r="C315">
-        <v>3423.79</v>
+        <v>3292.48</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316">
-        <f t="shared" si="2"/>
-        <v>2656.6399999999994</v>
-      </c>
-      <c r="B316">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2841.4699999999993</v>
       </c>
       <c r="C316">
-        <v>3534.2</v>
+        <v>3349.37</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317">
-        <f t="shared" si="2"/>
-        <v>2526.3899999999994</v>
+        <f t="shared" si="3"/>
+        <v>2767.0499999999993</v>
       </c>
       <c r="C317">
-        <v>3664.45</v>
+        <v>3423.79</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318">
-        <f t="shared" si="2"/>
-        <v>2523.5399999999991</v>
+        <f t="shared" si="3"/>
+        <v>2656.6399999999994</v>
+      </c>
+      <c r="B318">
+        <v>0</v>
       </c>
       <c r="C318">
-        <v>3667.3</v>
+        <v>3534.2</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319">
-        <f t="shared" si="2"/>
-        <v>2503.7399999999993</v>
-      </c>
-      <c r="B319">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2526.3899999999994</v>
       </c>
       <c r="C319">
-        <v>3687.1</v>
+        <v>3664.45</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320">
-        <f t="shared" si="2"/>
-        <v>2484.4499999999994</v>
+        <f t="shared" si="3"/>
+        <v>2523.5399999999991</v>
       </c>
       <c r="C320">
-        <v>3706.39</v>
+        <v>3667.3</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321">
-        <f t="shared" si="2"/>
-        <v>2481.0399999999991</v>
+        <f t="shared" si="3"/>
+        <v>2503.7399999999993</v>
+      </c>
+      <c r="B321">
+        <v>0</v>
       </c>
       <c r="C321">
-        <v>3709.8</v>
+        <v>3687.1</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322">
-        <f t="shared" si="2"/>
-        <v>2350.7399999999993</v>
-      </c>
-      <c r="B322">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2484.4499999999994</v>
       </c>
       <c r="C322">
-        <v>3840.1</v>
+        <v>3706.39</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323">
-        <f t="shared" si="2"/>
-        <v>2267.9899999999993</v>
-      </c>
-      <c r="B323">
-        <v>0.55000000000000004</v>
+        <f t="shared" si="3"/>
+        <v>2481.0399999999991</v>
       </c>
       <c r="C323">
-        <v>3922.85</v>
+        <v>3709.8</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324">
-        <f t="shared" si="2"/>
-        <v>2209.9399999999991</v>
+        <f t="shared" si="3"/>
+        <v>2350.7399999999993</v>
+      </c>
+      <c r="B324">
+        <v>0</v>
       </c>
       <c r="C324">
-        <v>3980.9</v>
+        <v>3840.1</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325">
-        <f t="shared" si="2"/>
-        <v>2196.9399999999991</v>
+        <f t="shared" si="3"/>
+        <v>2267.9899999999993</v>
       </c>
       <c r="B325">
-        <v>0.56000000000000005</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C325">
-        <v>3993.9</v>
+        <v>3922.85</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326">
-        <f t="shared" si="2"/>
-        <v>2192.9899999999993</v>
+        <f t="shared" si="3"/>
+        <v>2209.9399999999991</v>
       </c>
       <c r="C326">
-        <v>3997.85</v>
+        <v>3980.9</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327">
-        <f t="shared" si="2"/>
-        <v>2148.7399999999993</v>
+        <f t="shared" si="3"/>
+        <v>2196.9399999999991</v>
+      </c>
+      <c r="B327">
+        <v>0.56000000000000005</v>
       </c>
       <c r="C327">
-        <v>4042.1</v>
+        <v>3993.9</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328">
-        <f t="shared" si="2"/>
-        <v>1994.0399999999991</v>
+        <f t="shared" si="3"/>
+        <v>2192.9899999999993</v>
       </c>
       <c r="C328">
-        <v>4196.8</v>
+        <v>3997.85</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329">
-        <f t="shared" si="2"/>
-        <v>1800.5899999999992</v>
+        <f t="shared" si="3"/>
+        <v>2148.7399999999993</v>
       </c>
       <c r="C329">
-        <v>4390.25</v>
+        <v>4042.1</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330">
-        <f t="shared" si="2"/>
-        <v>1749.6899999999996</v>
+        <f t="shared" si="3"/>
+        <v>1994.0399999999991</v>
       </c>
       <c r="C330">
-        <v>4441.1499999999996</v>
+        <v>4196.8</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331">
-        <f t="shared" si="2"/>
-        <v>1651.3899999999994</v>
+        <f t="shared" si="3"/>
+        <v>1800.5899999999992</v>
       </c>
       <c r="C331">
-        <v>4539.45</v>
+        <v>4390.25</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1749.6899999999996</v>
       </c>
       <c r="C332">
+        <v>4441.1499999999996</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <f t="shared" si="3"/>
+        <v>1651.3899999999994</v>
+      </c>
+      <c r="C333">
+        <v>4539.45</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>0</v>
+      </c>
+      <c r="C334">
         <v>6190.9650000000001</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B335">
+        <f>SUM(B3:B334)</f>
+        <v>322.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started inputting secondary gammas for main primary levels from Hurst PRC paper
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/tungsten.xlsx
+++ b/levelfiles/spreadsheet/tungsten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajbiffl\Documents\nrCascadeSim\levelfiles\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68679819-1408-4580-9DA6-C0E559F1178D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3DE286-261F-4AA6-B486-C2732ABE6373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="270" windowWidth="24330" windowHeight="15105" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="270" windowWidth="24330" windowHeight="15105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t>W-181</t>
   </si>
@@ -94,9 +94,6 @@
     <t>W-183</t>
   </si>
   <si>
-    <t>relative abundance (per 100)</t>
-  </si>
-  <si>
     <t>barns</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t>Egamma</t>
-  </si>
-  <si>
-    <t>transitions from Sn all dipole transitions</t>
   </si>
   <si>
     <t>to ground = 0.134</t>
@@ -210,6 +204,66 @@
   <si>
     <t>electric quadropole</t>
   </si>
+  <si>
+    <t>from Sn</t>
+  </si>
+  <si>
+    <t>from 1188</t>
+  </si>
+  <si>
+    <t>from 457.95</t>
+  </si>
+  <si>
+    <t>from 450.23</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>from 1440</t>
+  </si>
+  <si>
+    <t>from 726.27</t>
+  </si>
+  <si>
+    <t>from 529.42</t>
+  </si>
+  <si>
+    <t>from 0</t>
+  </si>
+  <si>
+    <t>from 113.4</t>
+  </si>
+  <si>
+    <t>from 250.72</t>
+  </si>
+  <si>
+    <t>from 365.55</t>
+  </si>
+  <si>
+    <t>from 385.19</t>
+  </si>
+  <si>
+    <t>data from https://escholarship.org/uc/item/26q2x5f0 and https://doi.org/10.1103/PhysRevC.89.014606</t>
+  </si>
+  <si>
+    <t>rel abundance (per 100)</t>
+  </si>
+  <si>
+    <t>mag quadropole?</t>
+  </si>
+  <si>
+    <t>PRC cross sxn (b)</t>
+  </si>
+  <si>
+    <t>from:</t>
+  </si>
+  <si>
+    <t>PRC (barns)</t>
+  </si>
+  <si>
+    <t>all below per 100</t>
+  </si>
 </sst>
 </file>
 
@@ -251,12 +305,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF896D"/>
+        <fgColor rgb="FFF15A41"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -286,11 +340,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -307,7 +441,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -345,6 +478,19 @@
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,6 +499,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF15A41"/>
       <color rgb="FFFF896D"/>
     </mruColors>
   </colors>
@@ -661,36 +808,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -848,26 +995,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J313"/>
+  <dimension ref="A1:Z313"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -885,10 +1035,20 @@
         <v>38.090000000000003</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -902,21 +1062,66 @@
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4">
         <v>685.73</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2">
+        <v>891.93</v>
+      </c>
+      <c r="L2">
+        <v>881.77</v>
+      </c>
+      <c r="M2">
+        <v>863.29</v>
+      </c>
+      <c r="N2">
+        <v>860.76</v>
+      </c>
+      <c r="O2">
+        <v>852.41</v>
+      </c>
+      <c r="P2">
+        <v>840.21</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>816.26</v>
+      </c>
+      <c r="R2">
+        <v>803.37</v>
+      </c>
+      <c r="S2">
+        <v>782.29</v>
+      </c>
+      <c r="T2">
+        <v>762.15</v>
+      </c>
+      <c r="U2">
+        <v>640.49</v>
+      </c>
+      <c r="V2">
+        <v>303.35000000000002</v>
+      </c>
+      <c r="W2">
+        <v>204.9</v>
+      </c>
+      <c r="X2">
+        <v>145.85</v>
+      </c>
+      <c r="Y2">
+        <v>77.290000000000006</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f t="shared" ref="A3:A66" si="0">$E$1 - C3</f>
         <v>5466.76</v>
@@ -941,9 +1146,59 @@
       <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>39</v>
+      </c>
+      <c r="O3">
+        <v>82</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>14</v>
+      </c>
+      <c r="S3">
+        <v>69</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>22</v>
+      </c>
+      <c r="V3">
+        <v>66</v>
+      </c>
+      <c r="W3">
+        <v>100</v>
+      </c>
+      <c r="X3">
+        <v>100</v>
+      </c>
+      <c r="Y3">
+        <v>100</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f t="shared" si="0"/>
         <v>5389.4710000000005</v>
@@ -957,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="2"/>
@@ -966,38 +1221,114 @@
       <c r="G4" s="5"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="J4" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>33</v>
+      </c>
+      <c r="N4">
+        <v>39</v>
+      </c>
+      <c r="O4">
+        <v>88</v>
+      </c>
+      <c r="P4">
+        <v>28</v>
+      </c>
+      <c r="Q4">
+        <v>43</v>
+      </c>
+      <c r="R4">
+        <v>26</v>
+      </c>
+      <c r="S4">
+        <v>1.5</v>
+      </c>
+      <c r="U4">
+        <v>14</v>
+      </c>
+      <c r="V4">
+        <v>100</v>
+      </c>
+      <c r="W4">
+        <v>75</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>5320.9120000000003</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>0.60499999999999998</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>145.84800000000001</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <f t="shared" si="1"/>
         <v>1.5883433972171173</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="E5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="12">
         <f t="shared" si="2"/>
         <v>-539.88200000000006</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="2">
+        <v>1.625</v>
+      </c>
+      <c r="K5">
+        <v>44</v>
+      </c>
+      <c r="M5">
+        <v>21</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>33</v>
+      </c>
+      <c r="Q5">
+        <v>54</v>
+      </c>
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5">
+        <v>4.3</v>
+      </c>
+      <c r="T5">
+        <v>51</v>
+      </c>
+      <c r="V5">
+        <v>157.53</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>5265.3110000000006</v>
@@ -1011,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="2"/>
@@ -1021,39 +1352,92 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>11</v>
+      </c>
+      <c r="N6">
+        <v>44</v>
+      </c>
+      <c r="O6">
+        <v>7</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>5261.8580000000002</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>0.86</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>204.90199999999999</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" si="1"/>
         <v>2.2578104489367288</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="12">
         <f t="shared" si="2"/>
         <v>-480.82800000000003</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2.2970000000000002</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>34</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7">
+        <v>46</v>
+      </c>
+      <c r="P7">
+        <v>16</v>
+      </c>
+      <c r="Q7">
+        <v>68</v>
+      </c>
+      <c r="R7">
+        <v>19</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+      <c r="T7">
+        <v>100</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>5163.4070000000002</v>
@@ -1072,13 +1456,33 @@
         <v>-382.37700000000001</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <v>1.35E-2</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>1.8</v>
+      </c>
+      <c r="Q8">
+        <v>15</v>
+      </c>
+      <c r="R8">
+        <v>36</v>
+      </c>
+      <c r="V8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>5135.9800000000005</v>
@@ -1101,7 +1505,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>5116.3290000000006</v>
@@ -1120,13 +1524,28 @@
         <v>-335.29900000000004</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>14</v>
+      </c>
+      <c r="L10">
+        <v>94</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <v>13</v>
+      </c>
+      <c r="U10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>5102.54</v>
@@ -1148,8 +1567,11 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>5056.7</v>
@@ -1172,7 +1594,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>5034.4780000000001</v>
@@ -1194,8 +1616,20 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>1.7</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>32</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>4956.76</v>
@@ -1218,7 +1652,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>4944.6100000000006</v>
@@ -1241,7 +1675,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>4928.3100000000004</v>
@@ -1264,7 +1698,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>4892.71</v>
@@ -1287,7 +1721,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>4869.5200000000004</v>
@@ -1310,7 +1744,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>4853.38</v>
@@ -1333,7 +1767,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>4826.268</v>
@@ -1354,9 +1788,17 @@
       <c r="G20" s="5"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="2">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="U20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>4755.9800000000005</v>
@@ -1379,7 +1821,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>4738.9000000000005</v>
@@ -1402,7 +1844,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>4725.68</v>
@@ -1424,8 +1866,11 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>4704.607</v>
@@ -1444,13 +1889,18 @@
         <v>76.423000000000002</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="2">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="T24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>4691.16</v>
@@ -1473,36 +1923,40 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+    <row r="26" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>4684.47</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>0.15</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="12">
         <v>782.29</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <f t="shared" si="1"/>
         <v>0.39380414807035963</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="13">
+      <c r="F26" s="12">
         <f t="shared" si="2"/>
         <v>96.559999999999945</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="S26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>4669.7300000000005</v>
@@ -1525,7 +1979,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>4668.54</v>
@@ -1548,7 +2002,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>4663.3910000000005</v>
@@ -1569,9 +2023,14 @@
       <c r="G29" s="5"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="2">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="R29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>4656.97</v>
@@ -1590,13 +2049,13 @@
         <v>124.05999999999995</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>4655.0600000000004</v>
@@ -1619,7 +2078,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>4651.25</v>
@@ -1642,7 +2101,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>4650.5039999999999</v>
@@ -1663,34 +2122,44 @@
       <c r="G33" s="5"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="J33" s="2">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>4626.5550000000003</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="12">
         <v>0.124</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="12">
         <v>840.20500000000004</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="12">
         <f t="shared" si="1"/>
         <v>0.32554476240483066</v>
       </c>
       <c r="E34" s="5"/>
-      <c r="F34" s="13">
+      <c r="F34" s="12">
         <f t="shared" si="2"/>
         <v>154.47500000000002</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="2">
+        <v>0.627</v>
+      </c>
+      <c r="P34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <f t="shared" si="0"/>
         <v>4614.3500000000004</v>
@@ -1711,9 +2180,14 @@
       <c r="G35" s="5"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="2">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="O35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <f t="shared" si="0"/>
         <v>4606</v>
@@ -1734,9 +2208,14 @@
       <c r="G36" s="5"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="2">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="N36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>4603.47</v>
@@ -1757,9 +2236,14 @@
       <c r="G37" s="5"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="M37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>4600.08</v>
@@ -1782,7 +2266,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
         <v>4584.99</v>
@@ -1801,13 +2285,18 @@
         <v>196.03999999999996</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="2">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="L39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
         <v>4582.63</v>
@@ -1830,32 +2319,37 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+    <row r="41" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>4574.83</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="12">
         <v>0.152</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="12">
         <v>891.93</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="12">
         <f t="shared" si="1"/>
         <v>0.39905487004463108</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="F41" s="13">
+      <c r="F41" s="12">
         <f t="shared" si="2"/>
         <v>206.19999999999993</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="K41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
         <v>4565.76</v>
@@ -1878,7 +2372,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>4557.7800000000007</v>
@@ -1901,7 +2395,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>4555.96</v>
@@ -1924,7 +2418,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>4552.09</v>
@@ -1947,7 +2441,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>4533.76</v>
@@ -1970,7 +2464,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>4506.1900000000005</v>
@@ -1993,7 +2487,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>4501.8</v>
@@ -2104,7 +2598,7 @@
         <v>303.42999999999995</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -2175,7 +2669,7 @@
         <v>332.78</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -2453,7 +2947,7 @@
         <v>449.45000000000005</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2524,7 +3018,7 @@
         <v>506.77</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2549,7 +3043,7 @@
         <v>513.47</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -2602,22 +3096,22 @@
       <c r="J73" s="2"/>
     </row>
     <row r="74" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="13">
+      <c r="A74" s="12">
         <f t="shared" si="3"/>
         <v>4249.634</v>
       </c>
-      <c r="B74" s="13">
+      <c r="B74" s="12">
         <v>0.115</v>
       </c>
-      <c r="C74" s="13">
+      <c r="C74" s="12">
         <v>1217.126</v>
       </c>
-      <c r="D74" s="13">
+      <c r="D74" s="12">
         <f t="shared" si="4"/>
         <v>0.30191651352060905</v>
       </c>
       <c r="E74" s="5"/>
-      <c r="F74" s="13">
+      <c r="F74" s="12">
         <f t="shared" si="5"/>
         <v>531.39599999999996</v>
       </c>
@@ -2921,7 +3415,7 @@
         <v>642.97</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -4837,22 +5331,22 @@
       <c r="J170" s="2"/>
     </row>
     <row r="171" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="13">
+      <c r="A171" s="12">
         <f t="shared" si="6"/>
         <v>3469.57</v>
       </c>
-      <c r="B171" s="13">
+      <c r="B171" s="12">
         <v>0.10299999999999999</v>
       </c>
-      <c r="C171" s="13">
+      <c r="C171" s="12">
         <v>1997.19</v>
       </c>
-      <c r="D171" s="13">
+      <c r="D171" s="12">
         <f t="shared" si="7"/>
         <v>0.27041218167498027</v>
       </c>
       <c r="E171" s="5"/>
-      <c r="F171" s="13">
+      <c r="F171" s="12">
         <f t="shared" si="8"/>
         <v>1311.46</v>
       </c>
@@ -8102,7 +8596,7 @@
         <v>5.5972696245733795</v>
       </c>
       <c r="E313" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F313" s="5"/>
       <c r="G313" s="5"/>
@@ -8112,6 +8606,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8122,19 +8617,21 @@
   </sheetPr>
   <dimension ref="A1:I335"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.85546875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8157,72 +8654,71 @@
         <v>19.87</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="I1" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="6" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <f t="shared" ref="A3:A66" si="0">$E$1-C3</f>
         <v>6190.8399999999992</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>100</v>
       </c>
-      <c r="C3" s="14">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
         <v>0.45</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>6144.3561999999993</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>36.9</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>46.483800000000002</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.17399999999999999</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>20</v>
+      <c r="E4" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -8239,14 +8735,16 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -8260,7 +8758,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="2"/>
@@ -8280,7 +8778,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="2"/>
@@ -8449,7 +8947,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8917,17 +9415,17 @@
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
+      <c r="A46" s="12">
         <f t="shared" si="0"/>
         <v>5164.4669999999987</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="12">
         <v>36.299999999999997</v>
       </c>
-      <c r="C46" s="13">
+      <c r="C46" s="12">
         <v>1026.373</v>
       </c>
-      <c r="D46" s="13">
+      <c r="D46" s="12">
         <v>0.19</v>
       </c>
       <c r="E46" s="5"/>
@@ -11604,7 +12102,7 @@
         <v>2314.98</v>
       </c>
       <c r="D203" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E203" s="5"/>
       <c r="F203" s="2"/>
@@ -11674,7 +12172,7 @@
         <v>2349.6999999999998</v>
       </c>
       <c r="D207" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E207" s="5"/>
       <c r="F207" s="2"/>
@@ -13899,15 +14397,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14194,18 +14692,18 @@
   </sheetPr>
   <dimension ref="A1:I224"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15270,17 +15768,17 @@
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13">
+      <c r="A56" s="12">
         <f t="shared" si="0"/>
         <v>4572.3899999999994</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B56" s="12">
         <v>0.104</v>
       </c>
-      <c r="C56" s="13">
+      <c r="C56" s="12">
         <v>1181.3499999999999</v>
       </c>
-      <c r="D56" s="13">
+      <c r="D56" s="12">
         <f t="shared" si="2"/>
         <v>6.1248527679623086</v>
       </c>
@@ -17657,26 +18155,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="10" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="9" customWidth="1"/>
+    <col min="11" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17696,9 +18196,11 @@
         <v>21.67</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -17711,15 +18213,44 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f t="shared" ref="A3:A94" si="0">$E$1-C3</f>
         <v>6669.0199999999995</v>
@@ -17732,15 +18263,24 @@
         <f>100*B3/$G$1</f>
         <v>0</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="8" t="s">
+      <c r="E3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="30">
+        <v>13.39</v>
+      </c>
+      <c r="I3" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f t="shared" si="0"/>
         <v>6555.62</v>
@@ -17750,13 +18290,17 @@
         <v>113.4</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="31"/>
+      <c r="H4" s="30">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>6418.2999999999993</v>
@@ -17766,13 +18310,15 @@
         <v>250.72</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>6303.4699999999993</v>
@@ -17782,13 +18328,29 @@
         <v>365.55</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="33">
+        <v>1.74E-3</v>
+      </c>
+      <c r="K6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M6">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="N6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>6283.83</v>
@@ -17798,13 +18360,30 @@
         <v>385.19</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7">
+        <v>0.371</v>
+      </c>
+      <c r="M7">
+        <v>2.1099999999999999E-3</v>
+      </c>
+      <c r="N7">
+        <v>0.219</v>
+      </c>
+      <c r="O7">
+        <v>0.3</v>
+      </c>
+      <c r="P7">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>6259.7899999999991</v>
@@ -17819,8 +18398,11 @@
       <c r="G8" s="5"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>6254.7199999999993</v>
@@ -17836,49 +18418,67 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+    <row r="10" spans="1:16" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <f t="shared" si="0"/>
         <v>6218.9</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="20">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19">
         <v>450.12</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="23">
         <v>5.0999999999999997E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="L10" s="23">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M10" s="23">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <f t="shared" si="0"/>
         <v>6211.1799999999994</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="20">
+      <c r="B11" s="20"/>
+      <c r="C11" s="19">
         <v>457.84</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="23">
         <v>0.24299999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="23">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="N11" s="23">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>6193.4199999999992</v>
@@ -17893,8 +18493,11 @@
       <c r="G12" s="5"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1.43E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>6180.5899999999992</v>
@@ -17909,8 +18512,14 @@
       <c r="G13" s="5"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>6140.4199999999992</v>
@@ -17926,28 +18535,37 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:10" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+    <row r="15" spans="1:16" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
         <f t="shared" si="0"/>
         <v>6139.5999999999995</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="20">
+      <c r="B15" s="20"/>
+      <c r="C15" s="19">
         <v>529.41999999999996</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21" t="s">
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="23">
         <v>0.30399999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="23">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M15" s="23">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>6108.5899999999992</v>
@@ -17962,8 +18580,14 @@
       <c r="G16" s="5"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M16">
+        <v>6.6E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>6069.62</v>
@@ -17979,7 +18603,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>6059.82</v>
@@ -17995,7 +18619,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>6025.99</v>
@@ -18011,7 +18635,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>6007.3499999999995</v>
@@ -18027,7 +18651,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>5993.82</v>
@@ -18043,7 +18667,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>5954.0199999999995</v>
@@ -18059,28 +18683,31 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+    <row r="23" spans="1:13" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
         <f t="shared" si="0"/>
         <v>5942.75</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="20">
+      <c r="B23" s="20"/>
+      <c r="C23" s="19">
         <v>726.27</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="24">
+      <c r="J23" s="23">
         <v>2.4E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>5907.32</v>
@@ -18096,7 +18723,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>5885.0199999999995</v>
@@ -18112,7 +18739,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>5863.7199999999993</v>
@@ -18128,7 +18755,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>5861.5099999999993</v>
@@ -18143,8 +18770,11 @@
       <c r="G27" s="5"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>5854.82</v>
@@ -18160,7 +18790,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>5820.82</v>
@@ -18176,7 +18806,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>5732.0199999999995</v>
@@ -18192,7 +18822,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>5715.57</v>
@@ -18207,8 +18837,11 @@
       <c r="G31" s="5"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>5693.7199999999993</v>
@@ -18224,585 +18857,594 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
         <f t="shared" si="0"/>
         <v>5675.5199999999995</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <v>993.5</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
         <f t="shared" si="0"/>
         <v>5659.7</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <v>1009.32</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
         <f t="shared" si="0"/>
         <v>5630.0199999999995</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <v>1039</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
         <f t="shared" si="0"/>
         <v>5622.7199999999993</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <v>1046.3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
         <f t="shared" si="0"/>
         <v>5585.0199999999995</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <v>1084</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
         <f t="shared" si="0"/>
         <v>5582.23</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <v>1086.79</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="K38">
+        <v>2.9780000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
         <f t="shared" si="0"/>
         <v>5545.0199999999995</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <v>1124</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25">
+    <row r="40" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24">
         <f t="shared" si="0"/>
         <v>5480.69</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="24">
         <v>1188.33</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21" t="s">
+      <c r="D40" s="21"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="24">
+      <c r="J40" s="23">
         <v>3.5999999999999997E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="L40" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
         <f t="shared" si="0"/>
         <v>5476.0199999999995</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8">
         <v>1193</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
         <f t="shared" si="0"/>
         <v>5420.17</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <v>1248.8499999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
         <f t="shared" si="0"/>
         <v>5407.0199999999995</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8">
         <v>1262</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
         <f t="shared" si="0"/>
         <v>5400.82</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8">
         <v>1268.2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
         <f t="shared" si="0"/>
         <v>5397.0399999999991</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8">
         <v>1271.98</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
         <f t="shared" si="0"/>
         <v>5395.0199999999995</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="8">
         <v>1274</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
         <f t="shared" si="0"/>
         <v>5358.82</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8">
         <v>1310.2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
         <f t="shared" si="0"/>
         <v>5351.0199999999995</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8">
         <v>1318</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
         <f t="shared" si="0"/>
         <v>5339.1299999999992</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="8">
         <v>1329.89</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
         <f t="shared" si="0"/>
         <v>5313.7199999999993</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8">
         <v>1355.3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
         <f t="shared" si="0"/>
         <v>5303.42</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8">
         <v>1365.6</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
         <f t="shared" si="0"/>
         <v>5300.0199999999995</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="8">
         <v>1369</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
         <f t="shared" si="0"/>
         <v>5291.2699999999995</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="8">
         <v>1377.75</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
         <f t="shared" si="0"/>
         <v>5246.2199999999993</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="8">
         <v>1422.8</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="25">
+    <row r="55" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="24">
         <f t="shared" si="0"/>
         <v>5228.4699999999993</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="25">
+      <c r="B55" s="20"/>
+      <c r="C55" s="24">
         <v>1440.55</v>
       </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J55" s="24">
+      <c r="D55" s="21"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J55" s="23">
         <v>0.105</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="K55" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
         <f t="shared" si="0"/>
         <v>5199.91</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8">
         <v>1469.11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
         <f t="shared" si="0"/>
         <v>5170.8799999999992</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="8">
         <v>1498.14</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
         <f t="shared" si="0"/>
         <v>5167.0199999999995</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="8">
         <v>1502</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
         <f t="shared" si="0"/>
         <v>5156.119999999999</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8">
         <v>1512.9</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
         <f t="shared" si="0"/>
         <v>5150.5199999999995</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8">
         <v>1518.5</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
         <f t="shared" si="0"/>
         <v>5131.0199999999995</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8">
         <v>1538</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
         <f t="shared" si="0"/>
         <v>5108.7199999999993</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8">
         <v>1560.3</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
         <f t="shared" si="0"/>
         <v>5017.0199999999995</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="8">
         <v>1652</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
         <f t="shared" si="0"/>
         <v>5015.92</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C64" s="8">
         <v>1653.1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="A65" s="8">
         <f t="shared" si="0"/>
         <v>5002.0199999999995</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C65" s="8">
         <v>1667</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="A66" s="8">
         <f t="shared" si="0"/>
         <v>4957.0199999999995</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8">
         <v>1712</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="A67" s="8">
         <f t="shared" si="0"/>
         <v>4924.119999999999</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8">
         <v>1744.9</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="8">
         <f t="shared" si="0"/>
         <v>4891.82</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8">
         <v>1777.2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+      <c r="A69" s="8">
         <f t="shared" si="0"/>
         <v>4805.0199999999995</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <v>1864</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
+      <c r="A70" s="8">
         <f t="shared" si="0"/>
         <v>4777.0199999999995</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C70" s="8">
         <v>1892</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+      <c r="A71" s="8">
         <f t="shared" si="0"/>
         <v>4769.7199999999993</v>
       </c>
-      <c r="C71" s="9">
+      <c r="C71" s="8">
         <v>1899.3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+      <c r="A72" s="8">
         <f t="shared" si="0"/>
         <v>4724.0199999999995</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C72" s="8">
         <v>1945</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
+      <c r="A73" s="8">
         <f t="shared" si="0"/>
         <v>4674.119999999999</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C73" s="8">
         <v>1994.9</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+      <c r="A74" s="8">
         <f t="shared" si="0"/>
         <v>4654.0199999999995</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C74" s="8">
         <v>2015</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
+      <c r="A75" s="8">
         <f t="shared" si="0"/>
         <v>4635.0199999999995</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="8">
         <v>2034</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+      <c r="A76" s="8">
         <f t="shared" si="0"/>
         <v>4607.42</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="8">
         <v>2061.6</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+      <c r="A77" s="8">
         <f t="shared" si="0"/>
         <v>4602.0199999999995</v>
       </c>
-      <c r="C77" s="9">
+      <c r="C77" s="8">
         <v>2067</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
+      <c r="A78" s="8">
         <f t="shared" si="0"/>
         <v>4513.2199999999993</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C78" s="8">
         <v>2155.8000000000002</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+      <c r="A79" s="8">
         <f t="shared" si="0"/>
         <v>4398.119999999999</v>
       </c>
-      <c r="C79" s="9">
+      <c r="C79" s="8">
         <v>2270.9</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
+      <c r="A80" s="8">
         <f t="shared" si="0"/>
         <v>4099.119999999999</v>
       </c>
-      <c r="C80" s="9">
+      <c r="C80" s="8">
         <v>2569.9</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+      <c r="A81" s="8">
         <f t="shared" si="0"/>
         <v>4091.6199999999994</v>
       </c>
-      <c r="C81" s="9">
+      <c r="C81" s="8">
         <v>2577.4</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+      <c r="A82" s="8">
         <f t="shared" si="0"/>
         <v>3845.1199999999994</v>
       </c>
-      <c r="C82" s="9">
+      <c r="C82" s="8">
         <v>2823.9</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
+      <c r="A83" s="8">
         <f t="shared" si="0"/>
         <v>3778.1199999999994</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C83" s="8">
         <v>2890.9</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+      <c r="A84" s="8">
         <f t="shared" si="0"/>
         <v>3437.1199999999994</v>
       </c>
-      <c r="C84" s="9">
+      <c r="C84" s="8">
         <v>3231.9</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
+      <c r="A85" s="8">
         <f t="shared" si="0"/>
         <v>3104.1199999999994</v>
       </c>
-      <c r="C85" s="9">
+      <c r="C85" s="8">
         <v>3564.9</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
+      <c r="A86" s="8">
         <f t="shared" si="0"/>
         <v>3076.1199999999994</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C86" s="8">
         <v>3592.9</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+      <c r="A87" s="8">
         <f t="shared" si="0"/>
         <v>2725.1199999999994</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C87" s="8">
         <v>3943.9</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
+      <c r="A88" s="8">
         <f t="shared" si="0"/>
         <v>2295.0199999999995</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C88" s="8">
         <v>4374</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
+      <c r="A89" s="8">
         <f t="shared" si="0"/>
         <v>1429.0199999999995</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="8">
         <v>5240</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="9">
+      <c r="A90" s="8">
         <f t="shared" si="0"/>
         <v>529.01999999999953</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="8">
         <v>6140</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="9">
+      <c r="A91" s="8">
         <f t="shared" si="0"/>
         <v>-399.98000000000047</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="8">
         <v>7069</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="9">
+      <c r="A92" s="8">
         <f t="shared" si="0"/>
         <v>-1351.9800000000005</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="8">
         <v>8021</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="9">
+      <c r="A93" s="8">
         <f t="shared" si="0"/>
         <v>-1371.9800000000005</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="8">
         <v>8041</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="9">
+      <c r="A94" s="8">
         <f t="shared" si="0"/>
         <v>-1985.9800000000005</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <v>8655</v>
       </c>
     </row>

</xml_diff>